<commit_message>
moves with costs and attack and stuff, 15 spells in a table
</commit_message>
<xml_diff>
--- a/docs/moves 1.xlsx
+++ b/docs/moves 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="31">
   <si>
     <t xml:space="preserve">attack </t>
   </si>
@@ -78,6 +78,45 @@
   </si>
   <si>
     <t>staff slam</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>extras</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>2 block</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>2 block aoe</t>
+  </si>
+  <si>
+    <t>2 aoe</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>weapons</t>
+  </si>
+  <si>
+    <t>mana</t>
+  </si>
+  <si>
+    <t>extra</t>
   </si>
 </sst>
 </file>
@@ -121,6 +160,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1186,19 +1230,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:G80"/>
+  <dimension ref="D5:AT80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI22" sqref="AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:46" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>0</v>
       </c>
@@ -1208,84 +1258,606 @@
       <c r="G5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="4:46" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="4:46" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:46" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="T8" t="s">
+        <v>6</v>
+      </c>
+      <c r="U8">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
+        <v>20</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB8">
+        <v>2</v>
+      </c>
+      <c r="AC8">
+        <v>2</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE8">
+        <v>3</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+      <c r="AQ8">
+        <v>1</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:46" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>3</v>
+      </c>
+      <c r="W9" t="s">
+        <v>20</v>
+      </c>
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB9">
+        <v>4</v>
+      </c>
+      <c r="AC9">
+        <v>3</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE9">
+        <v>4</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI9">
+        <v>3</v>
+      </c>
+      <c r="AJ9">
+        <v>3</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL9">
+        <v>3</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ9">
+        <v>2</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="4:46" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="T10" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>4</v>
+      </c>
+      <c r="W10" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10">
+        <v>6</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB10">
+        <v>2</v>
+      </c>
+      <c r="AC10">
+        <v>4</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE10">
+        <v>6</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>3</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL10">
+        <v>6</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP10">
+        <v>4</v>
+      </c>
+      <c r="AQ10">
+        <v>4</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="4:46" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:46" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46">
+        <v>6</v>
+      </c>
+      <c r="I46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62">
+        <v>6</v>
+      </c>
+      <c r="I62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69" t="s">
+        <v>27</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74" t="s">
+        <v>27</v>
+      </c>
+      <c r="H74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
         <v>17</v>
       </c>
+      <c r="E80">
+        <v>4</v>
+      </c>
+      <c r="F80">
+        <v>4</v>
+      </c>
+      <c r="G80" t="s">
+        <v>27</v>
+      </c>
+      <c r="H80">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>